<commit_message>
Update graphs to clearer version
</commit_message>
<xml_diff>
--- a/Benchmarks/Benchmarks.xlsx
+++ b/Benchmarks/Benchmarks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\UDS\2018-01\Temps Reel\NXT-FTL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ecole\UDS\2018-01\Temps Reel\NXT-FTL\Benchmarks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B89CBE0E-58EF-44A5-B6CD-7AFD41DD031B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{2D2A7F93-5A95-4567-A7E8-574F47627E48}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{EC732793-55EE-4E02-8B2A-D244545C803D}"/>
   </bookViews>
@@ -182,8 +182,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-CA"/>
-              <a:t>Color</a:t>
+              <a:t>Temps de réponse en ms pour chaque lecture d'un capteur de</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="fr-CA" baseline="0"/>
+              <a:t> lumière</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CA"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -225,6 +230,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Couleur</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:noFill/>
@@ -1417,6 +1425,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Nombre de lectures</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1478,6 +1541,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Temps de réponse (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1599,8 +1717,13 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-CA"/>
-              <a:t>Distance</a:t>
+              <a:t>Temps de réponse en ms pour chaque lecture du</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="fr-CA" baseline="0"/>
+              <a:t> capteur de distance</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-CA"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -2273,6 +2396,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Nombre de lectures</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2334,6 +2512,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Temps de réponse (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2455,7 +2688,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-CA"/>
-              <a:t>Tacho</a:t>
+              <a:t>Temps de réponse en ms pour chaque lecture d'un moteur</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3690,6 +3923,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Nombre de lectures</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3751,6 +4039,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Temps de réponse (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3872,7 +4215,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-CA"/>
-              <a:t>Touch</a:t>
+              <a:t>Temps de réponse en ms pour chaque lecture du capteur de toucher</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4846,6 +5189,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Nombre de lectures</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4907,6 +5305,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-CA"/>
+                  <a:t>Temps de réponse (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -7222,15 +7675,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>19049</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>147636</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7258,15 +7711,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>138111</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>33337</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7293,16 +7746,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>128587</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>157162</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>128587</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7329,16 +7782,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>138112</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>138112</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>176212</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7367,23 +7820,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="motorFile" connectionId="3" xr16:uid="{00000000-0016-0000-0000-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="colorFile" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000004000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="touchFile" connectionId="5" xr16:uid="{00000000-0016-0000-0000-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="motorFile" connectionId="3" xr16:uid="{00000000-0016-0000-0000-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tachoFile" connectionId="4" xr16:uid="{00000000-0016-0000-0000-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="touchFile" connectionId="5" xr16:uid="{00000000-0016-0000-0000-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="distanceFile" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="tachoFile" connectionId="4" xr16:uid="{00000000-0016-0000-0000-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="colorFile" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="distanceFile" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7685,8 +8138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836BDA3C-EE0C-4FE2-9249-319D84283E72}">
   <dimension ref="A1:O379"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="E52" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>